<commit_message>
Thesis updated. Setup properties are updated.
</commit_message>
<xml_diff>
--- a/Papers/ICEM 2018/375W load frequency results/40000 msec freq 8+1_2.xlsx
+++ b/Papers/ICEM 2018/375W load frequency results/40000 msec freq 8+1_2.xlsx
@@ -2083,262 +2083,262 @@
                   <c:v>49.18</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>49.174999999999997</c:v>
+                  <c:v>49.17</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>49.172499999999999</c:v>
+                  <c:v>49.16</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>49.17</c:v>
+                  <c:v>49.15</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>49.17</c:v>
+                  <c:v>49.14</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1325</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>49.17</c:v>
+                  <c:v>49.125</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>49.17</c:v>
+                  <c:v>49.12</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>49.17</c:v>
+                  <c:v>49.115000000000002</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>49.17</c:v>
+                  <c:v>49.11</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>49.17</c:v>
+                  <c:v>49.104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>49.17</c:v>
+                  <c:v>49.102499999999999</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="277">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3043,112 +3043,112 @@
                   <c:v>49.18</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>49.174999999999997</c:v>
+                  <c:v>49.17</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>49.172499999999999</c:v>
+                  <c:v>49.16</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>49.17</c:v>
+                  <c:v>49.15</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>49.17</c:v>
+                  <c:v>49.14</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1325</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>49.17</c:v>
+                  <c:v>49.125</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>49.17</c:v>
+                  <c:v>49.12</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>49.17</c:v>
+                  <c:v>49.115000000000002</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>49.17</c:v>
+                  <c:v>49.11</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>49.17</c:v>
+                  <c:v>49.104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>49.17</c:v>
+                  <c:v>49.102499999999999</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>49.17</c:v>
+                  <c:v>49.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4900,8 +4900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="I272" sqref="I272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8999,7 +8999,7 @@
         <v>0.88762951388888889</v>
       </c>
       <c r="B194">
-        <v>49.174999999999997</v>
+        <v>49.17</v>
       </c>
       <c r="C194">
         <f t="shared" si="6"/>
@@ -9023,7 +9023,7 @@
         <v>0.88763212962962967</v>
       </c>
       <c r="B195">
-        <v>49.172499999999999</v>
+        <v>49.16</v>
       </c>
       <c r="C195">
         <f t="shared" ref="C195:C258" si="10">A195-0.887121666666667</f>
@@ -9047,7 +9047,7 @@
         <v>0.88763476851851852</v>
       </c>
       <c r="B196">
-        <v>49.17</v>
+        <v>49.15</v>
       </c>
       <c r="C196">
         <f t="shared" si="10"/>
@@ -9071,7 +9071,7 @@
         <v>0.88763765046296295</v>
       </c>
       <c r="B197">
-        <v>49.17</v>
+        <v>49.14</v>
       </c>
       <c r="C197">
         <f t="shared" si="10"/>
@@ -9095,7 +9095,7 @@
         <v>0.88764016203703699</v>
       </c>
       <c r="B198">
-        <v>49.17</v>
+        <v>49.1325</v>
       </c>
       <c r="C198">
         <f t="shared" si="10"/>
@@ -9119,7 +9119,7 @@
         <v>0.88764288194444452</v>
       </c>
       <c r="B199">
-        <v>49.17</v>
+        <v>49.125</v>
       </c>
       <c r="C199">
         <f t="shared" si="10"/>
@@ -9143,7 +9143,7 @@
         <v>0.88764557870370364</v>
       </c>
       <c r="B200">
-        <v>49.17</v>
+        <v>49.12</v>
       </c>
       <c r="C200">
         <f t="shared" si="10"/>
@@ -9167,7 +9167,7 @@
         <v>0.88764812500000001</v>
       </c>
       <c r="B201">
-        <v>49.17</v>
+        <v>49.115000000000002</v>
       </c>
       <c r="C201">
         <f t="shared" si="10"/>
@@ -9191,7 +9191,7 @@
         <v>0.88765079861111118</v>
       </c>
       <c r="B202">
-        <v>49.17</v>
+        <v>49.11</v>
       </c>
       <c r="C202">
         <f t="shared" si="10"/>
@@ -9215,7 +9215,7 @@
         <v>0.88765333333333329</v>
       </c>
       <c r="B203">
-        <v>49.17</v>
+        <v>49.104999999999997</v>
       </c>
       <c r="C203">
         <f t="shared" si="10"/>
@@ -9239,7 +9239,7 @@
         <v>0.88765603009259264</v>
       </c>
       <c r="B204">
-        <v>49.17</v>
+        <v>49.102499999999999</v>
       </c>
       <c r="C204">
         <f t="shared" si="10"/>
@@ -9263,7 +9263,7 @@
         <v>0.88765862268518525</v>
       </c>
       <c r="B205">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C205">
         <f t="shared" si="10"/>
@@ -9287,7 +9287,7 @@
         <v>0.8876611342592593</v>
       </c>
       <c r="B206">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C206">
         <f t="shared" si="10"/>
@@ -9311,7 +9311,7 @@
         <v>0.88766405092592582</v>
       </c>
       <c r="B207">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C207">
         <f t="shared" si="10"/>
@@ -9335,7 +9335,7 @@
         <v>0.88766650462962959</v>
       </c>
       <c r="B208">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C208">
         <f t="shared" si="10"/>
@@ -9359,7 +9359,7 @@
         <v>0.88766908564814806</v>
       </c>
       <c r="B209">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C209">
         <f t="shared" si="10"/>
@@ -9383,7 +9383,7 @@
         <v>0.88767194444444442</v>
       </c>
       <c r="B210">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C210">
         <f t="shared" si="10"/>
@@ -9407,7 +9407,7 @@
         <v>0.88767451388888885</v>
       </c>
       <c r="B211">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C211">
         <f t="shared" si="10"/>
@@ -9431,7 +9431,7 @@
         <v>0.88767718750000002</v>
       </c>
       <c r="B212">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C212">
         <f t="shared" si="10"/>
@@ -9455,7 +9455,7 @@
         <v>0.88767989583333329</v>
       </c>
       <c r="B213">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C213">
         <f t="shared" si="10"/>
@@ -9479,7 +9479,7 @@
         <v>0.88768230324074071</v>
       </c>
       <c r="B214">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C214">
         <f t="shared" si="10"/>
@@ -9503,7 +9503,7 @@
         <v>0.88768481481481487</v>
       </c>
       <c r="B215">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C215">
         <f t="shared" si="10"/>
@@ -9527,7 +9527,7 @@
         <v>0.88768748842592593</v>
       </c>
       <c r="B216">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C216">
         <f t="shared" si="10"/>
@@ -9551,7 +9551,7 @@
         <v>0.8876901041666666</v>
       </c>
       <c r="B217">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C217">
         <f t="shared" si="10"/>
@@ -9575,7 +9575,7 @@
         <v>0.88769298611111103</v>
       </c>
       <c r="B218">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C218">
         <f t="shared" si="10"/>
@@ -9599,7 +9599,7 @@
         <v>0.88769548611111115</v>
       </c>
       <c r="B219">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C219">
         <f t="shared" si="10"/>
@@ -9623,7 +9623,7 @@
         <v>0.88769836805555558</v>
       </c>
       <c r="B220">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C220">
         <f t="shared" si="10"/>
@@ -9647,7 +9647,7 @@
         <v>0.88770094907407404</v>
       </c>
       <c r="B221">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C221">
         <f t="shared" si="10"/>
@@ -9671,7 +9671,7 @@
         <v>0.88770343750000003</v>
       </c>
       <c r="B222">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C222">
         <f t="shared" si="10"/>
@@ -9695,7 +9695,7 @@
         <v>0.88770581018518513</v>
       </c>
       <c r="B223">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C223">
         <f t="shared" si="10"/>
@@ -9719,7 +9719,7 @@
         <v>0.8877083564814815</v>
       </c>
       <c r="B224">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C224">
         <f t="shared" si="10"/>
@@ -9743,7 +9743,7 @@
         <v>0.88771121527777774</v>
       </c>
       <c r="B225">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C225">
         <f t="shared" si="10"/>
@@ -9767,7 +9767,7 @@
         <v>0.88771391203703709</v>
       </c>
       <c r="B226">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C226">
         <f t="shared" si="10"/>
@@ -9791,7 +9791,7 @@
         <v>0.8877163194444444</v>
       </c>
       <c r="B227">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C227">
         <f t="shared" si="10"/>
@@ -9815,7 +9815,7 @@
         <v>0.88771899305555557</v>
       </c>
       <c r="B228">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C228">
         <f t="shared" si="10"/>
@@ -9839,7 +9839,7 @@
         <v>0.88772170138888884</v>
       </c>
       <c r="B229">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C229">
         <f t="shared" si="10"/>
@@ -9863,7 +9863,7 @@
         <v>0.88772405092592599</v>
       </c>
       <c r="B230">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C230">
         <f t="shared" si="10"/>
@@ -9883,7 +9883,7 @@
         <v>0.8877268055555555</v>
       </c>
       <c r="B231">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C231">
         <f t="shared" si="10"/>
@@ -9903,7 +9903,7 @@
         <v>0.88772946759259252</v>
       </c>
       <c r="B232">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C232">
         <f t="shared" si="10"/>
@@ -9923,7 +9923,7 @@
         <v>0.88773181712962967</v>
       </c>
       <c r="B233">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C233">
         <f t="shared" si="10"/>
@@ -9943,7 +9943,7 @@
         <v>0.88773452546296294</v>
       </c>
       <c r="B234">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C234">
         <f t="shared" si="10"/>
@@ -9963,7 +9963,7 @@
         <v>0.88773692129629633</v>
       </c>
       <c r="B235">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C235">
         <f t="shared" si="10"/>
@@ -9983,7 +9983,7 @@
         <v>0.8877395949074075</v>
       </c>
       <c r="B236">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C236">
         <f t="shared" si="10"/>
@@ -10003,7 +10003,7 @@
         <v>0.88774230324074077</v>
       </c>
       <c r="B237">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C237">
         <f t="shared" si="10"/>
@@ -10023,7 +10023,7 @@
         <v>0.88774467592592599</v>
       </c>
       <c r="B238">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C238">
         <f t="shared" si="10"/>
@@ -10043,7 +10043,7 @@
         <v>0.88774760416666665</v>
       </c>
       <c r="B239">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C239">
         <f t="shared" si="10"/>
@@ -10063,7 +10063,7 @@
         <v>0.88775045138888886</v>
       </c>
       <c r="B240">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C240">
         <f t="shared" si="10"/>
@@ -10083,7 +10083,7 @@
         <v>0.88775299768518512</v>
       </c>
       <c r="B241">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C241">
         <f t="shared" si="10"/>
@@ -10103,7 +10103,7 @@
         <v>0.88775585648148148</v>
       </c>
       <c r="B242">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C242">
         <f t="shared" si="10"/>
@@ -10123,7 +10123,7 @@
         <v>0.88775820601851851</v>
       </c>
       <c r="B243">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C243">
         <f t="shared" si="10"/>
@@ -10143,7 +10143,7 @@
         <v>0.88776093749999996</v>
       </c>
       <c r="B244">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C244">
         <f t="shared" si="10"/>
@@ -10163,7 +10163,7 @@
         <v>0.88776364583333323</v>
       </c>
       <c r="B245">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C245">
         <f t="shared" si="10"/>
@@ -10183,7 +10183,7 @@
         <v>0.88776606481481479</v>
       </c>
       <c r="B246">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C246">
         <f t="shared" si="10"/>
@@ -10203,7 +10203,7 @@
         <v>0.88776871527777779</v>
       </c>
       <c r="B247">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C247">
         <f t="shared" si="10"/>
@@ -10223,7 +10223,7 @@
         <v>0.88777122685185184</v>
       </c>
       <c r="B248">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C248">
         <f t="shared" si="10"/>
@@ -10243,7 +10243,7 @@
         <v>0.88777376157407406</v>
       </c>
       <c r="B249">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C249">
         <f t="shared" si="10"/>
@@ -10263,7 +10263,7 @@
         <v>0.88777634259259264</v>
       </c>
       <c r="B250">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C250">
         <f t="shared" si="10"/>
@@ -10283,7 +10283,7 @@
         <v>0.88777886574074072</v>
       </c>
       <c r="B251">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C251">
         <f t="shared" si="10"/>
@@ -10303,7 +10303,7 @@
         <v>0.88778160879629631</v>
       </c>
       <c r="B252">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C252">
         <f t="shared" si="10"/>
@@ -10323,7 +10323,7 @@
         <v>0.88778431712962957</v>
       </c>
       <c r="B253">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C253">
         <f t="shared" si="10"/>
@@ -10343,7 +10343,7 @@
         <v>0.88778679398148153</v>
       </c>
       <c r="B254">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C254">
         <f t="shared" si="10"/>
@@ -10363,7 +10363,7 @@
         <v>0.88778951388888894</v>
       </c>
       <c r="B255">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C255">
         <f t="shared" si="10"/>
@@ -10383,7 +10383,7 @@
         <v>0.88779202546296299</v>
       </c>
       <c r="B256">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C256">
         <f t="shared" si="10"/>
@@ -10403,7 +10403,7 @@
         <v>0.88779457175925935</v>
       </c>
       <c r="B257">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C257">
         <f t="shared" si="10"/>
@@ -10423,7 +10423,7 @@
         <v>0.88779728009259262</v>
       </c>
       <c r="B258">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C258">
         <f t="shared" si="10"/>
@@ -10443,7 +10443,7 @@
         <v>0.88779968749999993</v>
       </c>
       <c r="B259">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C259">
         <f t="shared" ref="C259:C279" si="14">A259-0.887121666666667</f>
@@ -10463,7 +10463,7 @@
         <v>0.88780239583333331</v>
       </c>
       <c r="B260">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C260">
         <f t="shared" si="14"/>
@@ -10483,7 +10483,7 @@
         <v>0.88780521990740746</v>
       </c>
       <c r="B261">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C261">
         <f t="shared" si="14"/>
@@ -10503,7 +10503,7 @@
         <v>0.88780759259259268</v>
       </c>
       <c r="B262">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C262">
         <f t="shared" si="14"/>
@@ -10523,7 +10523,7 @@
         <v>0.88781031249999998</v>
       </c>
       <c r="B263">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C263">
         <f t="shared" si="14"/>
@@ -10543,7 +10543,7 @@
         <v>0.88781265046296298</v>
       </c>
       <c r="B264">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C264">
         <f t="shared" si="14"/>
@@ -10563,7 +10563,7 @@
         <v>0.88781519675925924</v>
       </c>
       <c r="B265">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C265">
         <f t="shared" si="14"/>
@@ -10583,7 +10583,7 @@
         <v>0.88781773148148158</v>
       </c>
       <c r="B266">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C266">
         <f t="shared" si="14"/>
@@ -10603,7 +10603,7 @@
         <v>0.88782027777777772</v>
       </c>
       <c r="B267">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C267">
         <f t="shared" si="14"/>
@@ -10623,7 +10623,7 @@
         <v>0.88782278935185188</v>
       </c>
       <c r="B268">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C268">
         <f t="shared" si="14"/>
@@ -10643,7 +10643,7 @@
         <v>0.88782552083333333</v>
       </c>
       <c r="B269">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C269">
         <f t="shared" si="14"/>
@@ -10663,7 +10663,7 @@
         <v>0.88782806712962969</v>
       </c>
       <c r="B270">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C270">
         <f t="shared" si="14"/>
@@ -10683,7 +10683,7 @@
         <v>0.8878305671296296</v>
       </c>
       <c r="B271">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C271">
         <f t="shared" si="14"/>
@@ -10703,7 +10703,7 @@
         <v>0.88783292824074067</v>
       </c>
       <c r="B272">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C272">
         <f t="shared" si="14"/>
@@ -10723,7 +10723,7 @@
         <v>0.88783541666666677</v>
       </c>
       <c r="B273">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C273">
         <f t="shared" si="14"/>
@@ -10743,7 +10743,7 @@
         <v>0.88783813657407407</v>
       </c>
       <c r="B274">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C274">
         <f t="shared" si="14"/>
@@ -10763,7 +10763,7 @@
         <v>0.88784053240740735</v>
       </c>
       <c r="B275">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C275">
         <f t="shared" si="14"/>
@@ -10783,7 +10783,7 @@
         <v>0.88784307870370371</v>
       </c>
       <c r="B276">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C276">
         <f t="shared" si="14"/>
@@ -10803,7 +10803,7 @@
         <v>0.88784571759259256</v>
       </c>
       <c r="B277">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C277">
         <f t="shared" si="14"/>
@@ -10823,7 +10823,7 @@
         <v>0.88784826388888893</v>
       </c>
       <c r="B278">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C278">
         <f t="shared" si="14"/>
@@ -10843,7 +10843,7 @@
         <v>0.88785068287037039</v>
       </c>
       <c r="B279">
-        <v>49.17</v>
+        <v>49.1</v>
       </c>
       <c r="C279">
         <f t="shared" si="14"/>

</xml_diff>